<commit_message>
replcating indmom and lead_lag
</commit_message>
<xml_diff>
--- a/Factor_Investing2.xlsx
+++ b/Factor_Investing2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\longh\Desktop\factor_investing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28611C75-C884-47B3-B351-950E6CB6AF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A230A4-8AA0-4C7E-A4DB-0EB19B6F5059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{02E0D641-B0B4-49C8-9857-2531A299C902}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{02E0D641-B0B4-49C8-9857-2531A299C902}"/>
   </bookViews>
   <sheets>
     <sheet name="Volume" sheetId="1" r:id="rId1"/>
@@ -2229,31 +2229,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2576,8 +2576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52E0771-D44D-4699-BA30-D3904327EEF6}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="E16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2597,16 +2597,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="17" t="s">
         <v>272</v>
       </c>
@@ -2721,7 +2721,7 @@
       <c r="F5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="22" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="21" t="s">
@@ -2748,7 +2748,7 @@
       <c r="F6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="20"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="23"/>
@@ -2767,7 +2767,7 @@
       <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
       <c r="J7" s="23"/>
@@ -2788,7 +2788,7 @@
       <c r="F8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="20"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="23"/>
@@ -2872,7 +2872,7 @@
       <c r="F11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="22" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="21" t="s">
@@ -2881,7 +2881,7 @@
       <c r="I11" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="J11" s="22" t="s">
+      <c r="J11" s="20" t="s">
         <v>133</v>
       </c>
       <c r="K11" s="3"/>
@@ -2901,10 +2901,10 @@
       <c r="F12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="20"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
-      <c r="J12" s="22"/>
+      <c r="J12" s="20"/>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -2983,7 +2983,7 @@
       <c r="F15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="22" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="21" t="s">
@@ -3012,7 +3012,7 @@
       <c r="F16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="20"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
       <c r="J16" s="23"/>
@@ -3033,14 +3033,14 @@
       <c r="F17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="20"/>
+      <c r="G17" s="22"/>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
       <c r="J17" s="23"/>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="19">
+      <c r="A18" s="25">
         <v>2006</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -3052,22 +3052,22 @@
       <c r="F18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="J18" s="22" t="s">
+      <c r="J18" s="20" t="s">
         <v>189</v>
       </c>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="3">
         <v>58</v>
       </c>
@@ -3080,10 +3080,10 @@
       <c r="F19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="20"/>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -3213,18 +3213,6 @@
   </sheetData>
   <autoFilter ref="A2:L23" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="21">
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="G5:G8"/>
-    <mergeCell ref="H5:H8"/>
-    <mergeCell ref="I5:I8"/>
-    <mergeCell ref="J5:J8"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:J17"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="G18:G19"/>
@@ -3234,6 +3222,18 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="G5:G8"/>
+    <mergeCell ref="H5:H8"/>
+    <mergeCell ref="I5:I8"/>
+    <mergeCell ref="J5:J8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J10" r:id="rId1" xr:uid="{E980445D-0030-4E0C-9981-32473E6B087E}"/>
@@ -3264,8 +3264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92D51052-FB65-48AC-B9F8-6C9F831E27DA}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27:I28"/>
+    <sheetView tabSelected="1" topLeftCell="E28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3332,7 +3332,7 @@
       <c r="F2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="26" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="21" t="s">
@@ -3341,7 +3341,7 @@
       <c r="I2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="20" t="s">
         <v>33</v>
       </c>
       <c r="K2"/>
@@ -3359,10 +3359,10 @@
       <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="24"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
-      <c r="J3" s="22"/>
+      <c r="J3" s="20"/>
       <c r="K3"/>
     </row>
     <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -3378,10 +3378,10 @@
       <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="21"/>
       <c r="I4" s="21"/>
-      <c r="J4" s="22"/>
+      <c r="J4" s="20"/>
       <c r="K4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3397,10 +3397,10 @@
       <c r="F5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="24"/>
+      <c r="G5" s="26"/>
       <c r="H5" s="21"/>
       <c r="I5" s="21"/>
-      <c r="J5" s="22"/>
+      <c r="J5" s="20"/>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -3416,10 +3416,10 @@
       <c r="F6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="24"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
-      <c r="J6" s="22"/>
+      <c r="J6" s="20"/>
       <c r="K6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3437,10 +3437,10 @@
       <c r="F7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="24"/>
+      <c r="G7" s="26"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
+      <c r="J7" s="20"/>
       <c r="K7"/>
     </row>
     <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -3458,7 +3458,7 @@
       <c r="F8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="26" t="s">
         <v>18</v>
       </c>
       <c r="H8" s="21" t="s">
@@ -3467,7 +3467,7 @@
       <c r="I8" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="20" t="s">
         <v>53</v>
       </c>
       <c r="K8"/>
@@ -3485,10 +3485,10 @@
       <c r="F9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="24"/>
+      <c r="G9" s="26"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
-      <c r="J9" s="22"/>
+      <c r="J9" s="20"/>
       <c r="K9"/>
     </row>
     <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -3504,10 +3504,10 @@
       <c r="F10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="24"/>
+      <c r="G10" s="26"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
-      <c r="J10" s="22"/>
+      <c r="J10" s="20"/>
       <c r="K10"/>
     </row>
     <row r="11" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -3525,10 +3525,10 @@
       <c r="F11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="24"/>
+      <c r="G11" s="26"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
-      <c r="J11" s="22"/>
+      <c r="J11" s="20"/>
       <c r="K11"/>
     </row>
     <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -3544,10 +3544,10 @@
       <c r="F12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="24"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
-      <c r="J12" s="22"/>
+      <c r="J12" s="20"/>
       <c r="K12"/>
     </row>
     <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -3565,10 +3565,10 @@
       <c r="F13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="24"/>
+      <c r="G13" s="26"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
-      <c r="J13" s="22"/>
+      <c r="J13" s="20"/>
       <c r="K13"/>
     </row>
     <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -3586,7 +3586,7 @@
       <c r="F14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="22" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="21" t="s">
@@ -3595,7 +3595,7 @@
       <c r="I14" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="J14" s="22" t="s">
+      <c r="J14" s="20" t="s">
         <v>80</v>
       </c>
       <c r="K14"/>
@@ -3613,10 +3613,10 @@
       <c r="F15" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="20"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
-      <c r="J15" s="22"/>
+      <c r="J15" s="20"/>
       <c r="K15"/>
     </row>
     <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -3632,10 +3632,10 @@
       <c r="F16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="20"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
-      <c r="J16" s="22"/>
+      <c r="J16" s="20"/>
       <c r="K16"/>
     </row>
     <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -3651,10 +3651,10 @@
       <c r="F17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="20"/>
+      <c r="G17" s="22"/>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
-      <c r="J17" s="22"/>
+      <c r="J17" s="20"/>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -3670,10 +3670,10 @@
       <c r="F18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="20"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
-      <c r="J18" s="22"/>
+      <c r="J18" s="20"/>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -3787,7 +3787,7 @@
       <c r="G22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="18" t="s">
         <v>143</v>
       </c>
       <c r="I22" s="3" t="s">
@@ -3818,7 +3818,7 @@
       <c r="G23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="26" t="s">
+      <c r="H23" s="19" t="s">
         <v>158</v>
       </c>
       <c r="I23" s="6" t="s">
@@ -3879,7 +3879,7 @@
       <c r="G25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="25" t="s">
+      <c r="H25" s="18" t="s">
         <v>203</v>
       </c>
       <c r="I25" s="3" t="s">
@@ -3910,7 +3910,7 @@
       <c r="G26" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="19" t="s">
         <v>212</v>
       </c>
       <c r="I26" s="6" t="s">
@@ -3938,7 +3938,7 @@
       <c r="F27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="24" t="s">
+      <c r="G27" s="26" t="s">
         <v>77</v>
       </c>
       <c r="H27" s="27" t="s">
@@ -3947,7 +3947,7 @@
       <c r="I27" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="J27" s="22" t="s">
+      <c r="J27" s="20" t="s">
         <v>219</v>
       </c>
       <c r="K27"/>
@@ -3967,10 +3967,10 @@
       <c r="F28" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="24"/>
+      <c r="G28" s="26"/>
       <c r="H28" s="27"/>
       <c r="I28" s="21"/>
-      <c r="J28" s="22"/>
+      <c r="J28" s="20"/>
       <c r="K28"/>
     </row>
     <row r="29" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -4063,26 +4063,26 @@
   </sheetData>
   <autoFilter ref="A1:L31" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="20">
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="H14:H18"/>
+    <mergeCell ref="I14:I18"/>
+    <mergeCell ref="J14:J18"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="I2:I7"/>
+    <mergeCell ref="J2:J7"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="G8:G13"/>
     <mergeCell ref="H8:H13"/>
     <mergeCell ref="I8:I13"/>
     <mergeCell ref="J8:J13"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="H2:H7"/>
-    <mergeCell ref="I2:I7"/>
-    <mergeCell ref="J2:J7"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="G14:G18"/>
-    <mergeCell ref="H14:H18"/>
-    <mergeCell ref="I14:I18"/>
-    <mergeCell ref="J14:J18"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="J27:J28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J33" r:id="rId1" display="http://www.jstor.org/stable/pdfplus/4622342.pdf" xr:uid="{7D104546-AFF7-4DD9-8CCB-09D62CFB737E}"/>
@@ -4102,9 +4102,10 @@
     <hyperlink ref="J26" r:id="rId15" xr:uid="{C45D5EED-5E9C-4C9D-AEFB-0235B5FF6FC7}"/>
     <hyperlink ref="J22" r:id="rId16" xr:uid="{136492DC-BA9A-4A42-8548-BB85BBF809B9}"/>
     <hyperlink ref="J20" r:id="rId17" xr:uid="{AD3EB0A7-0688-4DA2-B357-77AEAE4F81EA}"/>
+    <hyperlink ref="J29" r:id="rId18" xr:uid="{40C4E3B1-73E9-488D-BDEC-9E5F2703FF04}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId18"/>
+  <pageSetup orientation="landscape" r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -4271,7 +4272,7 @@
       <c r="F5" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="22" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="21" t="s">
@@ -4298,7 +4299,7 @@
       <c r="F6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="20"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="23"/>
@@ -4317,7 +4318,7 @@
       <c r="F7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
       <c r="J7" s="23"/>
@@ -4338,7 +4339,7 @@
       <c r="F8" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="G8" s="20"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="23"/>
@@ -4359,7 +4360,7 @@
       <c r="F9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="22" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="21" t="s">
@@ -4386,7 +4387,7 @@
       <c r="F10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="20"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="23"/>
@@ -4405,7 +4406,7 @@
       <c r="F11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="20"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="23"/>
@@ -4426,7 +4427,7 @@
       <c r="F12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="20"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
       <c r="J12" s="23"/>
@@ -4742,16 +4743,16 @@
   </sheetData>
   <autoFilter ref="A1:L22" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="10">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
+    <mergeCell ref="J9:J12"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="G5:G8"/>
     <mergeCell ref="H5:H8"/>
     <mergeCell ref="I5:I8"/>
     <mergeCell ref="J5:J8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="I9:I12"/>
-    <mergeCell ref="J9:J12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J24" r:id="rId1" display="http://www.jstor.org/stable/pdfplus/4622342.pdf" xr:uid="{B3D158A8-2442-4689-AE2E-076C45C0C8FF}"/>

</xml_diff>